<commit_message>
xls export geometry fix, added server power\health status
</commit_message>
<xml_diff>
--- a/dell/C1TN2S2_hwinvent_report_hw_passed.xml_report.xlsx
+++ b/dell/C1TN2S2_hwinvent_report_hw_passed.xml_report.xlsx
@@ -43,7 +43,7 @@
     <t>PCI device</t>
   </si>
   <si>
-    <t>System memory size</t>
+    <t>Memory tot.size</t>
   </si>
   <si>
     <t>Memory serial</t>
@@ -73,7 +73,7 @@
     <t>2CC8A96F</t>
   </si>
   <si>
-    <t>Memory module part number</t>
+    <t>Memory P/Ns</t>
   </si>
   <si>
     <t>Memory slot</t>
@@ -112,10 +112,10 @@
     <t>HDD fw</t>
   </si>
   <si>
-    <t>HDD slot population</t>
-  </si>
-  <si>
-    <t>PSU part number</t>
+    <t>HDD slot pop.</t>
+  </si>
+  <si>
+    <t>PSU P/Ns</t>
   </si>
   <si>
     <t>PSU serial</t>
@@ -498,15 +498,15 @@
     <col min="3" max="3" width="25.7109375" customWidth="1"/>
     <col min="4" max="4" width="9.7109375" customWidth="1"/>
     <col min="5" max="5" width="10.7109375" customWidth="1"/>
-    <col min="6" max="6" width="18.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
     <col min="7" max="7" width="13.7109375" customWidth="1"/>
-    <col min="8" max="8" width="25.7109375" customWidth="1"/>
+    <col min="8" max="8" width="11.7109375" customWidth="1"/>
     <col min="9" max="9" width="11.7109375" customWidth="1"/>
     <col min="10" max="10" width="10.7109375" customWidth="1"/>
     <col min="11" max="11" width="9.7109375" customWidth="1"/>
     <col min="12" max="12" width="6.7109375" customWidth="1"/>
-    <col min="13" max="13" width="19.7109375" customWidth="1"/>
-    <col min="14" max="14" width="15.7109375" customWidth="1"/>
+    <col min="13" max="13" width="13.7109375" customWidth="1"/>
+    <col min="14" max="14" width="8.7109375" customWidth="1"/>
     <col min="15" max="15" width="14.7109375" customWidth="1"/>
     <col min="16" max="16" width="9.7109375" customWidth="1"/>
     <col min="17" max="17" width="6.7109375" customWidth="1"/>

</xml_diff>